<commit_message>
Generator of job-offer implemented
</commit_message>
<xml_diff>
--- a/raw_sources/language_probabilites.xlsx
+++ b/raw_sources/language_probabilites.xlsx
@@ -1058,6 +1058,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1087,24 +1090,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>0.17299999999999999</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C2" s="4">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D2" s="4">
-        <v>0.17</v>
+        <v>0.25</v>
       </c>
       <c r="E2" s="4">
-        <v>0.13</v>
+        <v>0.25</v>
       </c>
       <c r="F2" s="4">
-        <v>0.06</v>
-      </c>
-      <c r="G2">
-        <v>6.7000000000000004E-2</v>
+        <v>0.15</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.08</v>
       </c>
       <c r="H2" s="4"/>
+      <c r="I2" s="4">
+        <f>SUM(B2:G2)</f>
+        <v>1</v>
+      </c>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1130,6 +1137,10 @@
         <v>0.90600000000000003</v>
       </c>
       <c r="H3" s="4"/>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I12" si="0">SUM(B3:G3)</f>
+        <v>1</v>
+      </c>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1137,24 +1148,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>0.7</v>
+        <v>0.08</v>
       </c>
       <c r="C4" s="4">
-        <v>0.14599999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="D4" s="4">
-        <v>8.6999999999999994E-2</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G4" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F4" s="4">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="G4">
-        <v>0.03</v>
-      </c>
       <c r="H4" s="4"/>
+      <c r="I4" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1180,6 +1195,10 @@
         <v>1.2E-2</v>
       </c>
       <c r="H5" s="4"/>
+      <c r="I5" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1205,6 +1224,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="H6" s="4"/>
+      <c r="I6" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1212,24 +1235,28 @@
         <v>1</v>
       </c>
       <c r="B7" s="4">
-        <v>0.7</v>
+        <v>0.08</v>
       </c>
       <c r="C7" s="4">
-        <v>0.14599999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="D7" s="4">
-        <v>8.6999999999999994E-2</v>
+        <v>0.5</v>
       </c>
       <c r="E7" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G7" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F7" s="4">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="G7">
-        <v>0.03</v>
-      </c>
       <c r="H7" s="4"/>
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1255,6 +1282,10 @@
         <v>0.03</v>
       </c>
       <c r="H8" s="4"/>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1280,6 +1311,10 @@
         <v>1.2E-2</v>
       </c>
       <c r="H9" s="4"/>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1305,6 +1340,10 @@
         <v>1.2E-2</v>
       </c>
       <c r="H10" s="4"/>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1330,6 +1369,10 @@
         <v>1.2E-2</v>
       </c>
       <c r="H11" s="4"/>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1355,6 +1398,10 @@
         <v>0.03</v>
       </c>
       <c r="H12" s="4"/>
+      <c r="I12" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J12" s="4"/>
     </row>
     <row r="21" spans="7:7" x14ac:dyDescent="0.3">

</xml_diff>